<commit_message>
fix: ipmi threshold data error and ipmi sensor number low/upper format issue
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -407,11 +407,6 @@
           <t>Die_CPU2</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="5" s="3">
       <c r="A5" s="1" t="inlineStr">
@@ -419,11 +414,6 @@
           <t>CPU1_VR_Temp</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="6" s="3">
       <c r="A6" s="1" t="inlineStr">
@@ -431,11 +421,6 @@
           <t>CPU2_VR_Temp</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="7" s="3">
       <c r="A7" s="1" t="inlineStr">
@@ -445,7 +430,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>entity id, UNC, UC</t>
+          <t xml:space="preserve">entity id, </t>
         </is>
       </c>
     </row>
@@ -457,7 +442,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>entity id, UNC, UC</t>
+          <t xml:space="preserve">entity id, </t>
         </is>
       </c>
     </row>
@@ -469,7 +454,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>entity id, UNC, UC</t>
+          <t xml:space="preserve">entity id, </t>
         </is>
       </c>
     </row>
@@ -481,7 +466,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sensor number, entity id, UNC, UC</t>
+          <t xml:space="preserve">entity id, </t>
         </is>
       </c>
     </row>
@@ -491,11 +476,6 @@
           <t>NIC_Temp</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>sensor number, UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="12" s="3">
       <c r="A12" s="1" t="inlineStr">
@@ -503,11 +483,6 @@
           <t>DIMM_A1_CPU1</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>sensor number, UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="13" s="3">
       <c r="A13" s="1" t="inlineStr">
@@ -515,11 +490,6 @@
           <t>DIMM_A2_CPU1</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>sensor number, UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="14" s="3">
       <c r="A14" s="1" t="inlineStr">
@@ -527,11 +497,6 @@
           <t>DIMM_B1_CPU1</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>sensor number, UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="15" s="3">
       <c r="A15" s="1" t="inlineStr">
@@ -539,11 +504,6 @@
           <t>DIMM_B2_CPU1</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>sensor number, UNC, UC</t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="16" s="3">
       <c r="A16" s="1" t="inlineStr">
@@ -565,7 +525,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -577,7 +537,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -589,7 +549,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -601,7 +561,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -613,7 +573,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -625,7 +585,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -637,7 +597,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -649,7 +609,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -661,7 +621,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -673,7 +633,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -685,7 +645,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -697,7 +657,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -709,7 +669,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -721,7 +681,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -733,7 +693,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -745,7 +705,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -757,7 +717,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -769,7 +729,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -781,7 +741,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -793,7 +753,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -805,7 +765,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -817,7 +777,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -829,7 +789,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -841,7 +801,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -853,7 +813,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -865,7 +825,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -877,7 +837,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -889,7 +849,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -901,7 +861,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -913,7 +873,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -925,7 +885,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -937,7 +897,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sensor name, sensor number, UNC, UC</t>
+          <t xml:space="preserve">Sensor name, sensor number, </t>
         </is>
       </c>
     </row>
@@ -949,7 +909,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Sensor name, sensor number, UNC, UC</t>
+          <t xml:space="preserve">Sensor name, sensor number, </t>
         </is>
       </c>
     </row>
@@ -961,7 +921,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -973,7 +933,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -985,7 +945,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -997,7 +957,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1009,7 +969,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1021,7 +981,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1033,7 +993,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1045,7 +1005,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1057,7 +1017,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1069,7 +1029,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1081,7 +1041,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1093,7 +1053,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>
@@ -1105,7 +1065,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t xml:space="preserve">sensor number, </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: ipmi sensor number get appear error from DIMM_C1_CPU1 start
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>sensor number, UNC, UC</t>
+          <t>UNC, UC</t>
         </is>
       </c>
     </row>
@@ -523,11 +523,6 @@
           <t>DIMM_C2_CPU1</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="18" s="3">
       <c r="A18" s="1" t="inlineStr">
@@ -535,11 +530,6 @@
           <t>DIMM_D1_CPU1</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="19" s="3">
       <c r="A19" s="1" t="inlineStr">
@@ -547,11 +537,6 @@
           <t>DIMM_D2_CPU1</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="20" s="3">
       <c r="A20" s="1" t="inlineStr">
@@ -559,11 +544,6 @@
           <t>DIMM_E1_CPU1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="21" s="3">
       <c r="A21" s="1" t="inlineStr">
@@ -571,11 +551,6 @@
           <t>DIMM_E2_CPU1</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="22" s="3">
       <c r="A22" s="1" t="inlineStr">
@@ -583,11 +558,6 @@
           <t>DIMM_F1_CPU1</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="23" s="3">
       <c r="A23" s="1" t="inlineStr">
@@ -595,11 +565,6 @@
           <t>DIMM_F2_CPU1</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="24" s="3">
       <c r="A24" s="1" t="inlineStr">
@@ -607,11 +572,6 @@
           <t>DIMM_A1_CPU2</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="25" s="3">
       <c r="A25" s="1" t="inlineStr">
@@ -619,11 +579,6 @@
           <t>DIMM_A2_CPU2</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="26" s="3">
       <c r="A26" s="1" t="inlineStr">
@@ -631,11 +586,6 @@
           <t>DIMM_B1_CPU2</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="27" s="3">
       <c r="A27" s="1" t="inlineStr">
@@ -643,11 +593,6 @@
           <t>DIMM_B2_CPU2</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="28" s="3">
       <c r="A28" s="1" t="inlineStr">
@@ -655,11 +600,6 @@
           <t>DIMM_C1_CPU2</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="29" s="3">
       <c r="A29" s="1" t="inlineStr">
@@ -667,11 +607,6 @@
           <t>DIMM_C2_CPU2</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="30" s="3">
       <c r="A30" s="1" t="inlineStr">
@@ -679,11 +614,6 @@
           <t>DIMM_D1_CPU2</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="31" s="3">
       <c r="A31" s="1" t="inlineStr">
@@ -691,11 +621,6 @@
           <t>DIMM_D2_CPU2</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="32" s="3">
       <c r="A32" s="1" t="inlineStr">
@@ -703,11 +628,6 @@
           <t>DIMM_E1_CPU2</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="33" s="3">
       <c r="A33" s="1" t="inlineStr">
@@ -715,11 +635,6 @@
           <t>DIMM_E2_CPU2</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="34" s="3">
       <c r="A34" s="1" t="inlineStr">
@@ -727,11 +642,6 @@
           <t>DIMM_F1_CPU2</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="35" s="3">
       <c r="A35" s="1" t="inlineStr">
@@ -739,11 +649,6 @@
           <t>DIMM_F2_CPU2</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="36" s="3">
       <c r="A36" s="1" t="inlineStr">
@@ -751,11 +656,6 @@
           <t>PCH_Temp</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="37" s="3">
       <c r="A37" s="1" t="inlineStr">
@@ -763,11 +663,6 @@
           <t>PSU0_Temp</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="38" s="3">
       <c r="A38" s="1" t="inlineStr">
@@ -775,11 +670,6 @@
           <t>PSU1_Temp</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="39" s="3">
       <c r="A39" s="1" t="inlineStr">
@@ -787,11 +677,6 @@
           <t>PCIe_Temp</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="40" s="3">
       <c r="A40" s="2" t="inlineStr">
@@ -799,11 +684,6 @@
           <t>P12V_AUX</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="41" s="3">
       <c r="A41" s="2" t="inlineStr">
@@ -811,11 +691,6 @@
           <t>P5V_AUX</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="42" s="3">
       <c r="A42" s="1" t="inlineStr">
@@ -823,11 +698,6 @@
           <t>P3V3_AUX</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="43" s="3">
       <c r="A43" s="2" t="inlineStr">
@@ -835,11 +705,6 @@
           <t>P1V8_PCH_AUX</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="44" s="3">
       <c r="A44" s="2" t="inlineStr">
@@ -847,11 +712,6 @@
           <t>PVNN_PCH_AUX</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="45" s="3">
       <c r="A45" s="2" t="inlineStr">
@@ -859,11 +719,6 @@
           <t>P1V05_PCH_AUX</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="46" s="3">
       <c r="A46" s="2" t="inlineStr">
@@ -871,11 +726,6 @@
           <t>P1V2_DDR_BMC</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="47" s="3">
       <c r="A47" s="2" t="inlineStr">
@@ -883,11 +733,6 @@
           <t>P1V15_BMC</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="48" s="3">
       <c r="A48" s="2" t="inlineStr">
@@ -897,7 +742,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sensor name, sensor number, </t>
+          <t xml:space="preserve">Sensor name, </t>
         </is>
       </c>
     </row>
@@ -909,7 +754,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sensor name, sensor number, </t>
+          <t xml:space="preserve">Sensor name, </t>
         </is>
       </c>
     </row>
@@ -919,11 +764,6 @@
           <t>P12V_STBY</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="51" s="3">
       <c r="A51" s="2" t="inlineStr">
@@ -931,11 +771,6 @@
           <t>P12V_PSU</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="52" s="3">
       <c r="A52" s="2" t="inlineStr">
@@ -943,11 +778,6 @@
           <t>P5V</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="53" s="3">
       <c r="A53" s="2" t="inlineStr">
@@ -955,11 +785,6 @@
           <t>P3V3</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="54" s="3">
       <c r="A54" s="2" t="inlineStr">
@@ -967,11 +792,6 @@
           <t>PSU0_VIN</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="55" s="3">
       <c r="A55" s="2" t="inlineStr">
@@ -979,11 +799,6 @@
           <t>PSU0_VOUT</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="56" s="3">
       <c r="A56" s="2" t="inlineStr">
@@ -991,11 +806,6 @@
           <t>PSU0_IIN</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="57" s="3">
       <c r="A57" s="2" t="inlineStr">
@@ -1003,11 +813,6 @@
           <t>PSU0_IOUT</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="58" s="3">
       <c r="A58" s="2" t="inlineStr">
@@ -1015,11 +820,6 @@
           <t>PSU0_PIN</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="59" s="3">
       <c r="A59" s="2" t="inlineStr">
@@ -1027,11 +827,6 @@
           <t>PSU0_POUT</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="60" s="3">
       <c r="A60" s="2" t="inlineStr">
@@ -1039,11 +834,6 @@
           <t>PSU1_VIN</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="61" s="3">
       <c r="A61" s="2" t="inlineStr">
@@ -1051,11 +841,6 @@
           <t>PSU1_VOUT</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
     </row>
     <row customHeight="1" ht="15" r="62" s="3">
       <c r="A62" s="2" t="inlineStr">
@@ -1063,11 +848,7 @@
           <t>PSU1_IIN</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sensor number, </t>
-        </is>
-      </c>
+      <c r="B62" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="15" r="63" s="3">
       <c r="A63" s="2" t="inlineStr">

</xml_diff>